<commit_message>
turn code to create plot into function
</commit_message>
<xml_diff>
--- a/data/subgroupresults.xlsx
+++ b/data/subgroupresults.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ufscbr-my.sharepoint.com/personal/tamires_martins_ufsc_br/Documents/PC LAB/martins2023/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ufscbr-my.sharepoint.com/personal/tamires_martins_ufsc_br/Documents/PROJETO_R_GITHUB/martins2023/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{C1C7C836-8328-450F-9C24-F0B29ADFBD41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC55DCE3-09A1-43E8-A55A-11A130583194}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{C1C7C836-8328-450F-9C24-F0B29ADFBD41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F06282DC-A45A-4A9D-9D6D-8C51A9775AE7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="124">
   <si>
     <t>Swiss</t>
   </si>
@@ -296,9 +296,6 @@
     <t>Both sexes</t>
   </si>
   <si>
-    <t>No info</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -435,6 +432,21 @@
   </si>
   <si>
     <t>PT15’ + T6’ + S4’</t>
+  </si>
+  <si>
+    <t>Sex not reported</t>
+  </si>
+  <si>
+    <t>Strain not reported</t>
+  </si>
+  <si>
+    <t>Light cycle not reported</t>
+  </si>
+  <si>
+    <t>Method not reported</t>
+  </si>
+  <si>
+    <t>Via not reported</t>
   </si>
 </sst>
 </file>
@@ -815,8 +827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="K94" sqref="K94"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,25 +848,25 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>21</v>
@@ -898,7 +910,7 @@
         <v>82.88</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K2" s="1">
         <v>2.0699999999999998</v>
@@ -933,7 +945,7 @@
         <v>78.89</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K3" s="1">
         <v>1.53</v>
@@ -968,7 +980,7 @@
         <v>43.15</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K4" s="1">
         <v>0.28000000000000003</v>
@@ -1003,13 +1015,13 @@
         <v>82.35</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K5" s="1">
         <v>3.71</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>52</v>
       </c>
@@ -1020,7 +1032,7 @@
         <v>55</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>73</v>
+        <v>119</v>
       </c>
       <c r="E6" s="2">
         <v>7.26</v>
@@ -1038,7 +1050,7 @@
         <v>98.01</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K6" s="1">
         <v>33.08</v>
@@ -1073,7 +1085,7 @@
         <v>91.56</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K7" s="1">
         <v>6.05</v>
@@ -1108,7 +1120,7 @@
         <v>57.71</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K8" s="1">
         <v>0.64</v>
@@ -1143,7 +1155,7 @@
         <v>74.760000000000005</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K9" s="1">
         <v>0.68</v>
@@ -1178,7 +1190,7 @@
         <v>53.19</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K10" s="1">
         <v>0.4</v>
@@ -1213,7 +1225,7 @@
         <v>99.09</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K11" s="1">
         <v>77.52</v>
@@ -1248,7 +1260,7 @@
         <v>87.57</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K12" s="1">
         <v>12.37</v>
@@ -1283,7 +1295,7 @@
         <v>71.52</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K13" s="1">
         <v>0.67</v>
@@ -1318,7 +1330,7 @@
         <v>87.86</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K14" s="1">
         <v>2.41</v>
@@ -1353,7 +1365,7 @@
         <v>38.24</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K15" s="1">
         <v>0.2</v>
@@ -1388,13 +1400,13 @@
         <v>26.81</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K16" s="1">
         <v>0.52</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>52</v>
       </c>
@@ -1405,7 +1417,7 @@
         <v>58</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E17" s="2">
         <v>6.87</v>
@@ -1423,7 +1435,7 @@
         <v>88.55</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K17" s="1">
         <v>15.72</v>
@@ -1458,7 +1470,7 @@
         <v>0</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K18" s="1">
         <v>0</v>
@@ -1493,7 +1505,7 @@
         <v>26.9</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K19" s="1">
         <v>0.11</v>
@@ -1507,10 +1519,10 @@
         <v>53</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E20" s="2">
         <v>1.86</v>
@@ -1528,7 +1540,7 @@
         <v>85.87</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K20" s="1">
         <v>2.5</v>
@@ -1542,10 +1554,10 @@
         <v>53</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="E21" s="2">
         <v>1.82</v>
@@ -1563,7 +1575,7 @@
         <v>82.4</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K21" s="1">
         <v>2.0099999999999998</v>
@@ -1598,7 +1610,7 @@
         <v>65.77</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K22" s="1">
         <v>0.75</v>
@@ -1633,7 +1645,7 @@
         <v>87.38</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K23" s="1">
         <v>3.55</v>
@@ -1650,7 +1662,7 @@
         <v>59</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E24" s="2">
         <v>8.06</v>
@@ -1668,13 +1680,13 @@
         <v>99.36</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K24" s="1">
         <v>68.11</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>52</v>
       </c>
@@ -1685,7 +1697,7 @@
         <v>59</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>73</v>
+        <v>121</v>
       </c>
       <c r="E25" s="2">
         <v>3.24</v>
@@ -1703,7 +1715,7 @@
         <v>95.41</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K25" s="1">
         <v>7.95</v>
@@ -1738,7 +1750,7 @@
         <v>79.72</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K26" s="1">
         <v>1.53</v>
@@ -1773,7 +1785,7 @@
         <v>77.510000000000005</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K27" s="1">
         <v>1.32</v>
@@ -1808,7 +1820,7 @@
         <v>88.75</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K28" s="1">
         <v>2.79</v>
@@ -1843,13 +1855,13 @@
         <v>97.67</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K29" s="1">
         <v>64.7</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>52</v>
       </c>
@@ -1860,7 +1872,7 @@
         <v>55</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>73</v>
+        <v>119</v>
       </c>
       <c r="E30" s="2">
         <v>2.2599999999999998</v>
@@ -1878,7 +1890,7 @@
         <v>80.930000000000007</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K30" s="1">
         <v>2.65</v>
@@ -1913,7 +1925,7 @@
         <v>73.569999999999993</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K31" s="1">
         <v>1.19</v>
@@ -1948,7 +1960,7 @@
         <v>95.27</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K32" s="1">
         <v>7.84</v>
@@ -1983,7 +1995,7 @@
         <v>2.19</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K33" s="1">
         <v>1E-3</v>
@@ -2000,7 +2012,7 @@
         <v>58</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E34" s="2">
         <v>1.06</v>
@@ -2018,7 +2030,7 @@
         <v>48.7</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K34" s="1">
         <v>0.26</v>
@@ -2053,7 +2065,7 @@
         <v>63.96</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K35" s="1">
         <v>0.41</v>
@@ -2088,7 +2100,7 @@
         <v>19.73</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K36" s="1">
         <v>0.08</v>
@@ -2105,7 +2117,7 @@
         <v>58</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E37" s="2">
         <v>0.13</v>
@@ -2123,7 +2135,7 @@
         <v>40.96</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K37" s="1">
         <v>0.11</v>
@@ -2137,10 +2149,10 @@
         <v>54</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E38" s="2">
         <v>1.28</v>
@@ -2158,7 +2170,7 @@
         <v>72.099999999999994</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K38" s="1">
         <v>0.82</v>
@@ -2172,10 +2184,10 @@
         <v>54</v>
       </c>
       <c r="C39" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="E39" s="2">
         <v>1.53</v>
@@ -2193,7 +2205,7 @@
         <v>82.8</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K39" s="1">
         <v>2.0099999999999998</v>
@@ -2228,7 +2240,7 @@
         <v>74.92</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K40" s="1">
         <v>1.1599999999999999</v>
@@ -2263,13 +2275,13 @@
         <v>70.650000000000006</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K41" s="1">
         <v>1.01</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>52</v>
       </c>
@@ -2280,7 +2292,7 @@
         <v>59</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>73</v>
+        <v>121</v>
       </c>
       <c r="E42" s="2">
         <v>3.88</v>
@@ -2298,7 +2310,7 @@
         <v>97.36</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K42" s="1">
         <v>18.440000000000001</v>
@@ -2333,7 +2345,7 @@
         <v>74.98</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K43" s="1">
         <v>1.05</v>
@@ -2350,7 +2362,7 @@
         <v>59</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E44" s="2">
         <v>0.5</v>
@@ -2368,7 +2380,7 @@
         <v>36.26</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K44" s="1">
         <v>0.14000000000000001</v>
@@ -2403,7 +2415,7 @@
         <v>60.92</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K45" s="1">
         <v>1.37</v>
@@ -2438,7 +2450,7 @@
         <v>88.33</v>
       </c>
       <c r="J46" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K46" s="1">
         <v>3.14</v>
@@ -2455,7 +2467,7 @@
         <v>60</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E47" s="9">
         <v>3.7</v>
@@ -2473,7 +2485,7 @@
         <v>96.44</v>
       </c>
       <c r="J47" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K47" s="1">
         <v>14.22</v>
@@ -2490,7 +2502,7 @@
         <v>60</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E48" s="9">
         <v>1.47</v>
@@ -2508,7 +2520,7 @@
         <v>69.06</v>
       </c>
       <c r="J48" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K48" s="1">
         <v>0.88</v>
@@ -2525,7 +2537,7 @@
         <v>60</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E49" s="9">
         <v>1.21</v>
@@ -2543,7 +2555,7 @@
         <v>41.21</v>
       </c>
       <c r="J49" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K49" s="1">
         <v>0.17</v>
@@ -2560,7 +2572,7 @@
         <v>60</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E50" s="9">
         <v>0.05</v>
@@ -2578,7 +2590,7 @@
         <v>71.38</v>
       </c>
       <c r="J50" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K50" s="1">
         <v>0.63</v>
@@ -2595,7 +2607,7 @@
         <v>60</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E51" s="9">
         <v>1.29</v>
@@ -2613,7 +2625,7 @@
         <v>69.349999999999994</v>
       </c>
       <c r="J51" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K51" s="1">
         <v>1.1299999999999999</v>
@@ -2648,7 +2660,7 @@
         <v>83.32</v>
       </c>
       <c r="J52" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K52" s="1">
         <v>2.4</v>
@@ -2665,7 +2677,7 @@
         <v>61</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E53" s="9">
         <v>2.35</v>
@@ -2683,7 +2695,7 @@
         <v>85.72</v>
       </c>
       <c r="J53" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K53" s="1">
         <v>2.54</v>
@@ -2700,7 +2712,7 @@
         <v>61</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E54" s="9">
         <v>1.04</v>
@@ -2718,7 +2730,7 @@
         <v>0</v>
       </c>
       <c r="J54" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K54" s="1">
         <v>0</v>
@@ -2753,7 +2765,7 @@
         <v>84.11</v>
       </c>
       <c r="J55" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K55" s="1">
         <v>16.72</v>
@@ -2788,7 +2800,7 @@
         <v>59.16</v>
       </c>
       <c r="J56" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K56" s="1">
         <v>0.41</v>
@@ -2805,7 +2817,7 @@
         <v>61</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E57" s="9">
         <v>0.96</v>
@@ -2823,7 +2835,7 @@
         <v>68.28</v>
       </c>
       <c r="J57" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K57" s="1">
         <v>0.46</v>
@@ -2858,7 +2870,7 @@
         <v>88.39</v>
       </c>
       <c r="J58" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K58" s="1">
         <v>3.64</v>
@@ -2875,7 +2887,7 @@
         <v>62</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E59" s="9">
         <v>1.37</v>
@@ -2893,7 +2905,7 @@
         <v>0</v>
       </c>
       <c r="J59" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K59" s="1">
         <v>0</v>
@@ -2928,7 +2940,7 @@
         <v>79.66</v>
       </c>
       <c r="J60" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K60" s="1">
         <v>21.92</v>
@@ -2963,7 +2975,7 @@
         <v>32.75</v>
       </c>
       <c r="J61" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K61" s="1">
         <v>0.16</v>
@@ -2980,7 +2992,7 @@
         <v>63</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E62" s="9">
         <v>0.35</v>
@@ -2998,7 +3010,7 @@
         <v>0</v>
       </c>
       <c r="J62" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K62" s="1">
         <v>0</v>
@@ -3015,7 +3027,7 @@
         <v>63</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E63" s="9">
         <v>1.1499999999999999</v>
@@ -3033,7 +3045,7 @@
         <v>0</v>
       </c>
       <c r="J63" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K63" s="1">
         <v>0</v>
@@ -3050,7 +3062,7 @@
         <v>64</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E64" s="9">
         <v>0.63</v>
@@ -3068,7 +3080,7 @@
         <v>21.33</v>
       </c>
       <c r="J64" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K64" s="1">
         <v>0.17</v>
@@ -3103,7 +3115,7 @@
         <v>38.24</v>
       </c>
       <c r="J65" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K65" s="1">
         <v>0.18</v>
@@ -3120,7 +3132,7 @@
         <v>65</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E66" s="9">
         <v>1.42</v>
@@ -3138,7 +3150,7 @@
         <v>31.03</v>
       </c>
       <c r="J66" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K66" s="1">
         <v>0.21</v>
@@ -3155,7 +3167,7 @@
         <v>65</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E67" s="9">
         <v>0.33</v>
@@ -3173,7 +3185,7 @@
         <v>0</v>
       </c>
       <c r="J67" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K67" s="1">
         <v>0</v>
@@ -3208,7 +3220,7 @@
         <v>76.05</v>
       </c>
       <c r="J68" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K68" s="1">
         <v>1.44</v>
@@ -3243,7 +3255,7 @@
         <v>89.34</v>
       </c>
       <c r="J69" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K69" s="1">
         <v>3.32</v>
@@ -3260,7 +3272,7 @@
         <v>66</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E70" s="9">
         <v>2.42</v>
@@ -3278,7 +3290,7 @@
         <v>78.77</v>
       </c>
       <c r="J70" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K70" s="1">
         <v>1.66</v>
@@ -3295,7 +3307,7 @@
         <v>66</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E71" s="9">
         <v>0.17</v>
@@ -3313,13 +3325,13 @@
         <v>50.62</v>
       </c>
       <c r="J71" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K71" s="1">
         <v>0.3</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>56</v>
       </c>
@@ -3330,7 +3342,7 @@
         <v>66</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>73</v>
+        <v>123</v>
       </c>
       <c r="E72" s="9">
         <v>8.6999999999999993</v>
@@ -3348,7 +3360,7 @@
         <v>0</v>
       </c>
       <c r="J72" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K72" s="1">
         <v>0</v>
@@ -3383,7 +3395,7 @@
         <v>82.01</v>
       </c>
       <c r="J73" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K73" s="1">
         <v>1.98</v>
@@ -3400,7 +3412,7 @@
         <v>60</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E74" s="9">
         <v>2.64</v>
@@ -3418,7 +3430,7 @@
         <v>93.68</v>
       </c>
       <c r="J74" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K74" s="1">
         <v>6.88</v>
@@ -3435,7 +3447,7 @@
         <v>60</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E75" s="9">
         <v>1.19</v>
@@ -3453,7 +3465,7 @@
         <v>67.88</v>
       </c>
       <c r="J75" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K75" s="1">
         <v>0.7</v>
@@ -3470,7 +3482,7 @@
         <v>60</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E76" s="9">
         <v>1.28</v>
@@ -3488,7 +3500,7 @@
         <v>35.07</v>
       </c>
       <c r="J76" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K76" s="1">
         <v>0.44</v>
@@ -3505,7 +3517,7 @@
         <v>60</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E77" s="9">
         <v>0.2</v>
@@ -3523,7 +3535,7 @@
         <v>0</v>
       </c>
       <c r="J77" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K77" s="1">
         <v>0</v>
@@ -3558,7 +3570,7 @@
         <v>81</v>
       </c>
       <c r="J78" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K78" s="1">
         <v>1.42</v>
@@ -3575,7 +3587,7 @@
         <v>61</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E79" s="9">
         <v>1.65</v>
@@ -3593,7 +3605,7 @@
         <v>83.92</v>
       </c>
       <c r="J79" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K79" s="1">
         <v>1.91</v>
@@ -3610,7 +3622,7 @@
         <v>61</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E80" s="9">
         <v>2.09</v>
@@ -3628,7 +3640,7 @@
         <v>85.62</v>
       </c>
       <c r="J80" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K80" s="1">
         <v>2.46</v>
@@ -3645,7 +3657,7 @@
         <v>61</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E81" s="9">
         <v>0.2</v>
@@ -3663,7 +3675,7 @@
         <v>0.87</v>
       </c>
       <c r="J81" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K81" s="1">
         <v>2E-3</v>
@@ -3680,7 +3692,7 @@
         <v>61</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E82" s="9">
         <v>0.48</v>
@@ -3698,7 +3710,7 @@
         <v>0</v>
       </c>
       <c r="J82" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K82" s="1">
         <v>0</v>
@@ -3733,7 +3745,7 @@
         <v>18.559999999999999</v>
       </c>
       <c r="J83" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K83" s="1">
         <v>0.08</v>
@@ -3768,7 +3780,7 @@
         <v>71.95</v>
       </c>
       <c r="J84" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K84" s="1">
         <v>0.43</v>
@@ -3803,7 +3815,7 @@
         <v>54.84</v>
       </c>
       <c r="J85" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K85" s="1">
         <v>0.55000000000000004</v>
@@ -3820,7 +3832,7 @@
         <v>62</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E86" s="9">
         <v>1.21</v>
@@ -3838,7 +3850,7 @@
         <v>43.77</v>
       </c>
       <c r="J86" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K86" s="1">
         <v>0.48</v>
@@ -3855,7 +3867,7 @@
         <v>62</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E87" s="9">
         <v>2.86</v>
@@ -3873,7 +3885,7 @@
         <v>0</v>
       </c>
       <c r="J87" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K87" s="1">
         <v>0</v>
@@ -3890,7 +3902,7 @@
         <v>62</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E88" s="9">
         <v>0.55000000000000004</v>
@@ -3908,7 +3920,7 @@
         <v>0</v>
       </c>
       <c r="J88" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K88" s="1">
         <v>0</v>
@@ -3925,7 +3937,7 @@
         <v>62</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E89" s="9">
         <v>0.31</v>
@@ -3943,7 +3955,7 @@
         <v>43.96</v>
       </c>
       <c r="J89" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K89" s="1">
         <v>0.21</v>
@@ -3978,7 +3990,7 @@
         <v>79.069999999999993</v>
       </c>
       <c r="J90" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K90" s="1">
         <v>1.92</v>
@@ -3995,7 +4007,7 @@
         <v>65</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E91" s="9">
         <v>1.35</v>
@@ -4013,7 +4025,7 @@
         <v>82.54</v>
       </c>
       <c r="J91" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K91" s="1">
         <v>2.64</v>
@@ -4030,7 +4042,7 @@
         <v>65</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E92" s="9">
         <v>-0.36</v>
@@ -4048,7 +4060,7 @@
         <v>0</v>
       </c>
       <c r="J92" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K92" s="1">
         <v>0</v>
@@ -4062,10 +4074,10 @@
         <v>54</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E93" s="9">
         <v>2.52</v>
@@ -4083,7 +4095,7 @@
         <v>72.930000000000007</v>
       </c>
       <c r="J93" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K93" s="1">
         <v>2</v>
@@ -4118,7 +4130,7 @@
         <v>74.81</v>
       </c>
       <c r="J94" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K94" s="1">
         <v>1.19</v>
@@ -4153,7 +4165,7 @@
         <v>88.21</v>
       </c>
       <c r="J95" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K95" s="1">
         <v>3.14</v>
@@ -4170,7 +4182,7 @@
         <v>66</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E96" s="9">
         <v>1.44</v>
@@ -4188,7 +4200,7 @@
         <v>78.959999999999994</v>
       </c>
       <c r="J96" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K96" s="1">
         <v>1.1299999999999999</v>
@@ -4205,7 +4217,7 @@
         <v>66</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E97" s="9">
         <v>4.4800000000000004</v>
@@ -4223,7 +4235,7 @@
         <v>98.4</v>
       </c>
       <c r="J97" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K97" s="1">
         <v>32.61</v>
@@ -4240,7 +4252,7 @@
         <v>66</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E98" s="9">
         <v>1.1399999999999999</v>
@@ -4258,7 +4270,7 @@
         <v>0</v>
       </c>
       <c r="J98" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K98" s="1">
         <v>0</v>
@@ -4275,7 +4287,7 @@
         <v>66</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E99" s="9">
         <v>0.64</v>
@@ -4293,7 +4305,7 @@
         <v>79.23</v>
       </c>
       <c r="J99" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K99" s="1">
         <v>0.57999999999999996</v>
@@ -4328,7 +4340,7 @@
         <v>61</v>
       </c>
       <c r="J100" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K100" s="1">
         <v>1.46</v>
@@ -4345,7 +4357,7 @@
         <v>67</v>
       </c>
       <c r="D101" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E101" s="6">
         <v>1.63</v>
@@ -4363,7 +4375,7 @@
         <v>76.73</v>
       </c>
       <c r="J101" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K101" s="1">
         <v>1.19</v>
@@ -4398,7 +4410,7 @@
         <v>64.41</v>
       </c>
       <c r="J102" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K102" s="1">
         <v>1.22</v>
@@ -4415,7 +4427,7 @@
         <v>67</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E103" s="6">
         <v>5.57</v>
@@ -4433,7 +4445,7 @@
         <v>93.96</v>
       </c>
       <c r="J103" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K103" s="1">
         <v>20.76</v>
@@ -4468,7 +4480,7 @@
         <v>73.58</v>
       </c>
       <c r="J104" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K104" s="1">
         <v>0.7</v>
@@ -4503,7 +4515,7 @@
         <v>91.1</v>
       </c>
       <c r="J105" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K105" s="1">
         <v>4.17</v>
@@ -4538,7 +4550,7 @@
         <v>47.9</v>
       </c>
       <c r="J106" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K106" s="1">
         <v>0.68</v>
@@ -4573,7 +4585,7 @@
         <v>95.77</v>
       </c>
       <c r="J107" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K107" s="1">
         <v>69.25</v>
@@ -4590,7 +4602,7 @@
         <v>67</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E108" s="6">
         <v>0.83</v>
@@ -4608,7 +4620,7 @@
         <v>54.96</v>
       </c>
       <c r="J108" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K108" s="1">
         <v>0.7</v>
@@ -4625,7 +4637,7 @@
         <v>67</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E109" s="6">
         <v>0.41</v>
@@ -4643,7 +4655,7 @@
         <v>0</v>
       </c>
       <c r="J109" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K109" s="1">
         <v>0</v>
@@ -4660,7 +4672,7 @@
         <v>67</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E110" s="6">
         <v>2.79</v>
@@ -4678,7 +4690,7 @@
         <v>77.44</v>
       </c>
       <c r="J110" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K110" s="1">
         <v>1.1299999999999999</v>
@@ -4713,7 +4725,7 @@
         <v>38.24</v>
       </c>
       <c r="J111" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K111" s="1">
         <v>0.2</v>
@@ -4730,7 +4742,7 @@
         <v>67</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E112" s="9">
         <v>1.01</v>
@@ -4748,7 +4760,7 @@
         <v>0</v>
       </c>
       <c r="J112" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K112" s="1">
         <v>0</v>
@@ -4783,7 +4795,7 @@
         <v>79.150000000000006</v>
       </c>
       <c r="J113" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K113" s="1">
         <v>0.91</v>
@@ -4818,7 +4830,7 @@
         <v>26.87</v>
       </c>
       <c r="J114" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K114" s="1">
         <v>0.28999999999999998</v>
@@ -4853,13 +4865,13 @@
         <v>69.010000000000005</v>
       </c>
       <c r="J115" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K115" s="1">
         <v>0.44</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>57</v>
       </c>
@@ -4870,7 +4882,7 @@
         <v>68</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>73</v>
+        <v>122</v>
       </c>
       <c r="E116" s="9">
         <v>2.42</v>
@@ -4888,7 +4900,7 @@
         <v>88.29</v>
       </c>
       <c r="J116" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K116" s="1">
         <v>3.51</v>
@@ -4905,7 +4917,7 @@
         <v>68</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E117" s="9">
         <v>1.06</v>
@@ -4923,7 +4935,7 @@
         <v>67.95</v>
       </c>
       <c r="J117" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K117" s="1">
         <v>0.81</v>
@@ -4958,7 +4970,7 @@
         <v>94.95</v>
       </c>
       <c r="J118" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K118" s="1">
         <v>7.52</v>
@@ -4975,7 +4987,7 @@
         <v>69</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E119" s="9">
         <v>2.1</v>
@@ -4993,7 +5005,7 @@
         <v>82.05</v>
       </c>
       <c r="J119" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K119" s="1">
         <v>2.19</v>
@@ -5010,7 +5022,7 @@
         <v>69</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E120" s="9">
         <v>1.1499999999999999</v>
@@ -5028,7 +5040,7 @@
         <v>78</v>
       </c>
       <c r="J120" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K120" s="1">
         <v>1.17</v>
@@ -5063,7 +5075,7 @@
         <v>78.73</v>
       </c>
       <c r="J121" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K121" s="1">
         <v>1.48</v>
@@ -5098,7 +5110,7 @@
         <v>76.45</v>
       </c>
       <c r="J122" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K122" s="1">
         <v>1.17</v>
@@ -5133,7 +5145,7 @@
         <v>64.239999999999995</v>
       </c>
       <c r="J123" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K123" s="1">
         <v>0.56000000000000005</v>
@@ -5150,7 +5162,7 @@
         <v>67</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E124" s="9">
         <v>15.68</v>
@@ -5168,7 +5180,7 @@
         <v>24.84</v>
       </c>
       <c r="J124" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K124" s="1">
         <v>5.0599999999999996</v>
@@ -5203,7 +5215,7 @@
         <v>84.93</v>
       </c>
       <c r="J125" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K125" s="1">
         <v>2.38</v>
@@ -5238,7 +5250,7 @@
         <v>87.47</v>
       </c>
       <c r="J126" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K126" s="1">
         <v>3.48</v>
@@ -5255,7 +5267,7 @@
         <v>67</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E127" s="9">
         <v>1.73</v>
@@ -5273,13 +5285,13 @@
         <v>0</v>
       </c>
       <c r="J127" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K127" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>57</v>
       </c>
@@ -5290,7 +5302,7 @@
         <v>68</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>73</v>
+        <v>122</v>
       </c>
       <c r="E128" s="9">
         <v>1.89</v>
@@ -5308,7 +5320,7 @@
         <v>87.97</v>
       </c>
       <c r="J128" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K128" s="1">
         <v>3.46</v>
@@ -5325,7 +5337,7 @@
         <v>68</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E129" s="9">
         <v>1.0900000000000001</v>
@@ -5343,7 +5355,7 @@
         <v>71.38</v>
       </c>
       <c r="J129" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K129" s="1">
         <v>0.81</v>
@@ -5378,7 +5390,7 @@
         <v>85.34</v>
       </c>
       <c r="J130" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K130" s="1">
         <v>2.31</v>
@@ -5395,7 +5407,7 @@
         <v>69</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E131" s="9">
         <v>1.45</v>
@@ -5413,7 +5425,7 @@
         <v>79.09</v>
       </c>
       <c r="J131" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K131" s="1">
         <v>1.52</v>
@@ -5430,7 +5442,7 @@
         <v>69</v>
       </c>
       <c r="D132" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E132" s="2">
         <v>1.4</v>
@@ -5448,7 +5460,7 @@
         <v>82.53</v>
       </c>
       <c r="J132" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K132" s="1">
         <v>1.64</v>

</xml_diff>

<commit_message>
change via to route
</commit_message>
<xml_diff>
--- a/data/subgroupresults.xlsx
+++ b/data/subgroupresults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ufscbr-my.sharepoint.com/personal/tamires_martins_ufsc_br/Documents/PROJETO_R_GITHUB/martins2023/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{C1C7C836-8328-450F-9C24-F0B29ADFBD41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F06282DC-A45A-4A9D-9D6D-8C51A9775AE7}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{C1C7C836-8328-450F-9C24-F0B29ADFBD41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C73D65B6-6A70-42C5-94CA-46543E054D4C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -446,7 +446,7 @@
     <t>Method not reported</t>
   </si>
   <si>
-    <t>Via not reported</t>
+    <t>Route not reported</t>
   </si>
 </sst>
 </file>
@@ -827,7 +827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
       <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>

</xml_diff>